<commit_message>
CHANGE Miilon - Add more vocabulary to Unit 4.
</commit_message>
<xml_diff>
--- a/MiilonData/EditoB2_unite4_p59.xlsx
+++ b/MiilonData/EditoB2_unite4_p59.xlsx
@@ -9,10 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GÉNÉRALITÉS" sheetId="1" r:id="rId1"/>
+    <sheet name="POUR QUALIFIER UN LIEU" sheetId="2" r:id="rId2"/>
+    <sheet name="LOCALISATION" sheetId="3" r:id="rId3"/>
+    <sheet name="PAR RAPPORT À UN POINT" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="279">
   <si>
     <t>Mot français</t>
   </si>
@@ -333,6 +336,534 @@
   </si>
   <si>
     <t>sousedství</t>
+  </si>
+  <si>
+    <t>étendu, e</t>
+  </si>
+  <si>
+    <t>e.ta~dü</t>
+  </si>
+  <si>
+    <t>roztažený, rozprostřený, rozložený</t>
+  </si>
+  <si>
+    <t>immense</t>
+  </si>
+  <si>
+    <t>imma~:s</t>
+  </si>
+  <si>
+    <t>nesmírný, nekonečný, ohromný</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t>larž</t>
+  </si>
+  <si>
+    <t>široký, prostranný</t>
+  </si>
+  <si>
+    <t>minuscule</t>
+  </si>
+  <si>
+    <t>minüskül</t>
+  </si>
+  <si>
+    <t>maličký, nepatrný</t>
+  </si>
+  <si>
+    <t>spacieux, euse</t>
+  </si>
+  <si>
+    <t>spasjö, spasjö:z</t>
+  </si>
+  <si>
+    <t>prostorný</t>
+  </si>
+  <si>
+    <t>vaste</t>
+  </si>
+  <si>
+    <t>vast</t>
+  </si>
+  <si>
+    <t>rozsáhlý, prostranný, širý</t>
+  </si>
+  <si>
+    <t>à</t>
+  </si>
+  <si>
+    <t>prép</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>v, do</t>
+  </si>
+  <si>
+    <t>ailleurs</t>
+  </si>
+  <si>
+    <t>adv</t>
+  </si>
+  <si>
+    <t>ajö:r</t>
+  </si>
+  <si>
+    <t>jinde, jinam</t>
+  </si>
+  <si>
+    <t>en l'air</t>
+  </si>
+  <si>
+    <t>a~ le:r</t>
+  </si>
+  <si>
+    <t>do vzduchu, ve vzduchu, marně</t>
+  </si>
+  <si>
+    <t>en avant</t>
+  </si>
+  <si>
+    <t>a~ nava~</t>
+  </si>
+  <si>
+    <t>vpřed</t>
+  </si>
+  <si>
+    <t>d'un bout à l'autre</t>
+  </si>
+  <si>
+    <t>z jednoho kraje / konce na druhý</t>
+  </si>
+  <si>
+    <t>ça et là</t>
+  </si>
+  <si>
+    <t>sem a tam, sem tam</t>
+  </si>
+  <si>
+    <t>chez</t>
+  </si>
+  <si>
+    <t>še.</t>
+  </si>
+  <si>
+    <t>(doma) u, (do domu) k</t>
+  </si>
+  <si>
+    <t>dans</t>
+  </si>
+  <si>
+    <t>da~</t>
+  </si>
+  <si>
+    <t>v (uvnitř), do (dovnitř)</t>
+  </si>
+  <si>
+    <t>de tous côtés</t>
+  </si>
+  <si>
+    <t>ze všech stran</t>
+  </si>
+  <si>
+    <t>du côté ouest</t>
+  </si>
+  <si>
+    <t>dü ko.te. uest</t>
+  </si>
+  <si>
+    <t>d@ tu ko.te.</t>
+  </si>
+  <si>
+    <t>od západu</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>a~</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>à l'endroit</t>
+  </si>
+  <si>
+    <t>v místě, na místo</t>
+  </si>
+  <si>
+    <t>à l'envers</t>
+  </si>
+  <si>
+    <t>par endroits</t>
+  </si>
+  <si>
+    <t>par a~dru^a</t>
+  </si>
+  <si>
+    <t>místy</t>
+  </si>
+  <si>
+    <t>a la~ve:r</t>
+  </si>
+  <si>
+    <t>naruby, vzhůru nohama, naopak</t>
+  </si>
+  <si>
+    <t>ici</t>
+  </si>
+  <si>
+    <t>isi</t>
+  </si>
+  <si>
+    <t>zde, tady</t>
+  </si>
+  <si>
+    <t>là</t>
+  </si>
+  <si>
+    <t>la</t>
+  </si>
+  <si>
+    <t>tu</t>
+  </si>
+  <si>
+    <t>là-bas</t>
+  </si>
+  <si>
+    <t>laba</t>
+  </si>
+  <si>
+    <t>tam</t>
+  </si>
+  <si>
+    <t>n'import où</t>
+  </si>
+  <si>
+    <t>ne~portu</t>
+  </si>
+  <si>
+    <t>kdekoliv</t>
+  </si>
+  <si>
+    <t>nulle part</t>
+  </si>
+  <si>
+    <t>nül pa:r</t>
+  </si>
+  <si>
+    <t>nikde</t>
+  </si>
+  <si>
+    <t>partout</t>
+  </si>
+  <si>
+    <t>partu</t>
+  </si>
+  <si>
+    <t>všude</t>
+  </si>
+  <si>
+    <t>quelque part</t>
+  </si>
+  <si>
+    <t>kelk@ pa:r</t>
+  </si>
+  <si>
+    <t>někde</t>
+  </si>
+  <si>
+    <t>par terre</t>
+  </si>
+  <si>
+    <t>par te:r</t>
+  </si>
+  <si>
+    <t>na zemi, na zem, po zemi</t>
+  </si>
+  <si>
+    <t>à l'angle (de)</t>
+  </si>
+  <si>
+    <t>v úhlu / v rohu (čeho)</t>
+  </si>
+  <si>
+    <t>à l'arrière (de)</t>
+  </si>
+  <si>
+    <t>na zádi (čeho)</t>
+  </si>
+  <si>
+    <t>en arrière</t>
+  </si>
+  <si>
+    <t>vzadu, pozadu</t>
+  </si>
+  <si>
+    <t>au-delà de</t>
+  </si>
+  <si>
+    <t>za čím, na druhé straně čeho</t>
+  </si>
+  <si>
+    <t>autour (de)</t>
+  </si>
+  <si>
+    <t>kolem (čeho)</t>
+  </si>
+  <si>
+    <t>autre part</t>
+  </si>
+  <si>
+    <t>jinde</t>
+  </si>
+  <si>
+    <t>à l'avant (de)</t>
+  </si>
+  <si>
+    <t>na přídi (čeho)</t>
+  </si>
+  <si>
+    <t>en bas (de)</t>
+  </si>
+  <si>
+    <t>dole, v dolní části (čeho)</t>
+  </si>
+  <si>
+    <t>au bord (de)</t>
+  </si>
+  <si>
+    <t>na kraji (čeho)</t>
+  </si>
+  <si>
+    <t>au bout (de)</t>
+  </si>
+  <si>
+    <t>na konci (čeho)</t>
+  </si>
+  <si>
+    <t>au centre (de)</t>
+  </si>
+  <si>
+    <t>uprostřed (čeho)</t>
+  </si>
+  <si>
+    <t>au coin (de)</t>
+  </si>
+  <si>
+    <t>na rohu (čeho)</t>
+  </si>
+  <si>
+    <t>dans un coin</t>
+  </si>
+  <si>
+    <t>v rohu</t>
+  </si>
+  <si>
+    <t>sur le côté (de)</t>
+  </si>
+  <si>
+    <t>po straně / podél (čeho)</t>
+  </si>
+  <si>
+    <t>dedans</t>
+  </si>
+  <si>
+    <t>uvnitř</t>
+  </si>
+  <si>
+    <t>dehors</t>
+  </si>
+  <si>
+    <t>venku</t>
+  </si>
+  <si>
+    <t>en dehors de</t>
+  </si>
+  <si>
+    <t>vně čeho</t>
+  </si>
+  <si>
+    <t>au dehors de</t>
+  </si>
+  <si>
+    <t>kromě / mimo čeho</t>
+  </si>
+  <si>
+    <t>derrière</t>
+  </si>
+  <si>
+    <t>za, vzadu</t>
+  </si>
+  <si>
+    <t>dessous</t>
+  </si>
+  <si>
+    <t>pod</t>
+  </si>
+  <si>
+    <t>dole, dolů, vespod, spodní část, spodek</t>
+  </si>
+  <si>
+    <t>au-dessous (de)</t>
+  </si>
+  <si>
+    <t>pod (čím)</t>
+  </si>
+  <si>
+    <t>en dessous (de)</t>
+  </si>
+  <si>
+    <t>pod (čím), níže než (co)</t>
+  </si>
+  <si>
+    <t>par-dessous</t>
+  </si>
+  <si>
+    <t>ještě, více, dále, přes, kromě</t>
+  </si>
+  <si>
+    <t>devant</t>
+  </si>
+  <si>
+    <t>před</t>
+  </si>
+  <si>
+    <t>au devant de</t>
+  </si>
+  <si>
+    <t>naproti komu, vstříc komu</t>
+  </si>
+  <si>
+    <t>à (la) droite (de)</t>
+  </si>
+  <si>
+    <t>napravo od, vpravo</t>
+  </si>
+  <si>
+    <t>sur votre droite</t>
+  </si>
+  <si>
+    <t>po vaší pravici</t>
+  </si>
+  <si>
+    <t>entre</t>
+  </si>
+  <si>
+    <t>mezi</t>
+  </si>
+  <si>
+    <t>face à</t>
+  </si>
+  <si>
+    <t>proti čemu, naproti čemu</t>
+  </si>
+  <si>
+    <t>face à face</t>
+  </si>
+  <si>
+    <t>tváří v tvář</t>
+  </si>
+  <si>
+    <t>en face (de)</t>
+  </si>
+  <si>
+    <t>naproti (čemu)</t>
+  </si>
+  <si>
+    <t>au fond (de)</t>
+  </si>
+  <si>
+    <t>na dně (čeho)</t>
+  </si>
+  <si>
+    <t>à (la) gauche (de)</t>
+  </si>
+  <si>
+    <t>napravo do, vpravo</t>
+  </si>
+  <si>
+    <t>sur votre gauche</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> po vaší levici</t>
+  </si>
+  <si>
+    <t>en haut (de)</t>
+  </si>
+  <si>
+    <t>nahoře, nahoře na čem</t>
+  </si>
+  <si>
+    <t>de haut</t>
+  </si>
+  <si>
+    <t>seshora</t>
+  </si>
+  <si>
+    <t>hors de</t>
+  </si>
+  <si>
+    <t>mimo co</t>
+  </si>
+  <si>
+    <t>de là</t>
+  </si>
+  <si>
+    <t>odtud</t>
+  </si>
+  <si>
+    <t>par là</t>
+  </si>
+  <si>
+    <t>tudy</t>
+  </si>
+  <si>
+    <t>au milieu (de)</t>
+  </si>
+  <si>
+    <t>au pied de</t>
+  </si>
+  <si>
+    <t>na úpatí čeho</t>
+  </si>
+  <si>
+    <t>au sein de</t>
+  </si>
+  <si>
+    <t>uvnitř čeho, uprostřed čeho, v čem</t>
+  </si>
+  <si>
+    <t>au seuil de</t>
+  </si>
+  <si>
+    <t>na prahu čeho, na počátku čeho</t>
+  </si>
+  <si>
+    <t>sous</t>
+  </si>
+  <si>
+    <t>sur</t>
+  </si>
+  <si>
+    <t>nad, na</t>
+  </si>
+  <si>
+    <t>à la tête de</t>
+  </si>
+  <si>
+    <t>v čele čeho</t>
+  </si>
+  <si>
+    <t>en tête (de)</t>
+  </si>
+  <si>
+    <t>v čele, na počátku, v záhlaví čeho</t>
   </si>
 </sst>
 </file>
@@ -682,7 +1213,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1264,4 +1797,983 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="str">
+        <f xml:space="preserve"> "{ ""foreign"": """ &amp; A2 &amp; """, ""grammar"": """ &amp; B2 &amp; """, ""pronunciation"": """ &amp; C2 &amp; """, ""meaning"": """ &amp; D2 &amp; """ },"</f>
+        <v>{ "foreign": "étendu, e", "grammar": "adj", "pronunciation": "e.ta~dü", "meaning": "roztažený, rozprostřený, rozložený" },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F7" si="0" xml:space="preserve"> "{ ""foreign"": """ &amp; A3 &amp; """, ""grammar"": """ &amp; B3 &amp; """, ""pronunciation"": """ &amp; C3 &amp; """, ""meaning"": """ &amp; D3 &amp; """ },"</f>
+        <v>{ "foreign": "immense", "grammar": "adj", "pronunciation": "imma~:s", "meaning": "nesmírný, nekonečný, ohromný" },</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "large", "grammar": "adj", "pronunciation": "larž", "meaning": "široký, prostranný" },</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "minuscule", "grammar": "adj", "pronunciation": "minüskül", "meaning": "maličký, nepatrný" },</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "spacieux, euse", "grammar": "adj", "pronunciation": "spasjö, spasjö:z", "meaning": "prostorný" },</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "vaste", "grammar": "adj", "pronunciation": "vast", "meaning": "rozsáhlý, prostranný, širý" },</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" t="str">
+        <f xml:space="preserve"> "{ ""foreign"": """ &amp; A2 &amp; """, ""grammar"": """ &amp; B2 &amp; """, ""pronunciation"": """ &amp; C2 &amp; """, ""meaning"": """ &amp; D2 &amp; """ },"</f>
+        <v>{ "foreign": "à", "grammar": "prép", "pronunciation": "a", "meaning": "v, do" },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F23" si="0" xml:space="preserve"> "{ ""foreign"": """ &amp; A3 &amp; """, ""grammar"": """ &amp; B3 &amp; """, ""pronunciation"": """ &amp; C3 &amp; """, ""meaning"": """ &amp; D3 &amp; """ },"</f>
+        <v>{ "foreign": "ailleurs", "grammar": "adv", "pronunciation": "ajö:r", "meaning": "jinde, jinam" },</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "en l'air", "grammar": "adv", "pronunciation": "a~ le:r", "meaning": "do vzduchu, ve vzduchu, marně" },</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "en avant", "grammar": "adv", "pronunciation": "a~ nava~", "meaning": "vpřed" },</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "d'un bout à l'autre", "grammar": "", "pronunciation": "", "meaning": "z jednoho kraje / konce na druhý" },</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "ça et là", "grammar": "", "pronunciation": "", "meaning": "sem a tam, sem tam" },</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "chez", "grammar": "prép", "pronunciation": "še.", "meaning": "(doma) u, (do domu) k" },</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "dans", "grammar": "prép", "pronunciation": "da~", "meaning": "v (uvnitř), do (dovnitř)" },</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" t="s">
+        <v>146</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "de tous côtés", "grammar": "adv", "pronunciation": "d@ tu ko.te.", "meaning": "ze všech stran" },</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "du côté ouest", "grammar": "adv", "pronunciation": "dü ko.te. uest", "meaning": "od západu" },</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" t="s">
+        <v>153</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "en", "grammar": "prép", "pronunciation": "a~", "meaning": "v" },</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" t="s">
+        <v>155</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "à l'endroit", "grammar": "", "pronunciation": "", "meaning": "v místě, na místo" },</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D14" t="s">
+        <v>159</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "par endroits", "grammar": "adv", "pronunciation": "par a~dru^a", "meaning": "místy" },</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" t="s">
+        <v>161</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "à l'envers", "grammar": "adv", "pronunciation": "a la~ve:r", "meaning": "naruby, vzhůru nohama, naopak" },</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" t="s">
+        <v>164</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "ici", "grammar": "adv", "pronunciation": "isi", "meaning": "zde, tady" },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17" t="s">
+        <v>167</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "là", "grammar": "adv", "pronunciation": "la", "meaning": "tu" },</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" t="s">
+        <v>169</v>
+      </c>
+      <c r="D18" t="s">
+        <v>170</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "là-bas", "grammar": "adv", "pronunciation": "laba", "meaning": "tam" },</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" t="s">
+        <v>172</v>
+      </c>
+      <c r="D19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "n'import où", "grammar": "adv", "pronunciation": "ne~portu", "meaning": "kdekoliv" },</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" t="s">
+        <v>175</v>
+      </c>
+      <c r="D20" t="s">
+        <v>176</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "nulle part", "grammar": "adv", "pronunciation": "nül pa:r", "meaning": "nikde" },</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>177</v>
+      </c>
+      <c r="B21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" t="s">
+        <v>178</v>
+      </c>
+      <c r="D21" t="s">
+        <v>179</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "partout", "grammar": "adv", "pronunciation": "partu", "meaning": "všude" },</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" t="s">
+        <v>181</v>
+      </c>
+      <c r="D22" t="s">
+        <v>182</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "quelque part", "grammar": "adv", "pronunciation": "kelk@ pa:r", "meaning": "někde" },</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" t="s">
+        <v>184</v>
+      </c>
+      <c r="D23" t="s">
+        <v>185</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "par terre", "grammar": "adv", "pronunciation": "par te:r", "meaning": "na zemi, na zem, po zemi" },</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F2" t="str">
+        <f xml:space="preserve"> "{ ""foreign"": """ &amp; A2 &amp; """, ""grammar"": """ &amp; B2 &amp; """, ""pronunciation"": """ &amp; C2 &amp; """, ""meaning"": """ &amp; D2 &amp; """ },"</f>
+        <v>{ "foreign": "à l'angle (de)", "grammar": "", "pronunciation": "", "meaning": "v úhlu / v rohu (čeho)" },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>198</v>
+      </c>
+      <c r="D8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>202</v>
+      </c>
+      <c r="D10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>206</v>
+      </c>
+      <c r="D12" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D15" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>214</v>
+      </c>
+      <c r="D16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>216</v>
+      </c>
+      <c r="D17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>220</v>
+      </c>
+      <c r="D18" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>218</v>
+      </c>
+      <c r="D19" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>222</v>
+      </c>
+      <c r="D20" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>224</v>
+      </c>
+      <c r="D21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>227</v>
+      </c>
+      <c r="D22" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>229</v>
+      </c>
+      <c r="D23" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>231</v>
+      </c>
+      <c r="D24" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>233</v>
+      </c>
+      <c r="D26" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>237</v>
+      </c>
+      <c r="D28" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>239</v>
+      </c>
+      <c r="D29" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>241</v>
+      </c>
+      <c r="D30" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>243</v>
+      </c>
+      <c r="D31" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>245</v>
+      </c>
+      <c r="D32" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>247</v>
+      </c>
+      <c r="D33" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>249</v>
+      </c>
+      <c r="D34" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>251</v>
+      </c>
+      <c r="D35" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>253</v>
+      </c>
+      <c r="D36" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>255</v>
+      </c>
+      <c r="D37" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>257</v>
+      </c>
+      <c r="D38" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>259</v>
+      </c>
+      <c r="D39" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>261</v>
+      </c>
+      <c r="D40" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>263</v>
+      </c>
+      <c r="D41" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>265</v>
+      </c>
+      <c r="D42" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>266</v>
+      </c>
+      <c r="D43" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>268</v>
+      </c>
+      <c r="D44" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>270</v>
+      </c>
+      <c r="D45" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>272</v>
+      </c>
+      <c r="D46" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>273</v>
+      </c>
+      <c r="D47" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>275</v>
+      </c>
+      <c r="D48" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>277</v>
+      </c>
+      <c r="D49" t="s">
+        <v>278</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>